<commit_message>
Dev : Completed all layers DAG dev except NULLs counts Doc : Updated PL Mapping sheet
</commit_message>
<xml_diff>
--- a/mapping_sheets/presentation_layer_mapping.xlsx
+++ b/mapping_sheets/presentation_layer_mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CANCELLATION" sheetId="1" state="visible" r:id="rId2"/>
@@ -167,6 +167,7 @@
         <color rgb="FF000000"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">SELECT DISTINCT ORIGIN_AIRPORT_SEQ_ID AIRPORT_CODE,SPLIT(UPPER(ORIGIN_CITY_NAME),',')[0] CITY_NAME
 FROM </t>
@@ -177,6 +178,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">INTEGRATION_LAYER</t>
     </r>
@@ -186,6 +188,7 @@
         <color rgb="FF000000"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.FLIGHTS
 UNION
@@ -198,6 +201,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">INTEGRATION_LAYER</t>
     </r>
@@ -207,6 +211,7 @@
         <color rgb="FF000000"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.FLIGHTS</t>
     </r>
@@ -251,6 +256,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">year(</t>
     </r>
@@ -260,6 +266,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">'DATE'</t>
     </r>
@@ -269,6 +276,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -283,6 +291,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">month(</t>
     </r>
@@ -292,6 +301,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">'DATE'</t>
     </r>
@@ -301,6 +311,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -315,6 +326,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">dayofmonth(</t>
     </r>
@@ -324,6 +336,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">'DATE'</t>
     </r>
@@ -333,6 +346,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -350,6 +364,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">dayofyear(</t>
     </r>
@@ -359,6 +374,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">'DATE'</t>
     </r>
@@ -368,6 +384,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -382,6 +399,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">date_format(</t>
     </r>
@@ -391,6 +409,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">'DATE'</t>
     </r>
@@ -400,6 +419,7 @@
         <color rgb="FFCC7832"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, </t>
     </r>
@@ -409,6 +429,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">'E'</t>
     </r>
@@ -418,6 +439,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -631,7 +653,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -681,36 +703,28 @@
       <color rgb="FF333333"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFA9B7C6"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC7832"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -805,7 +819,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -813,11 +827,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -900,8 +914,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -991,7 +1005,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
@@ -1066,17 +1080,17 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="84.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.19"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1194,7 +1208,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1292,7 +1306,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1359,7 +1373,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>33</v>
@@ -1508,9 +1522,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="21.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="49.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="49.8"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="8" width="11.52"/>
   </cols>
   <sheetData>
@@ -1644,7 +1658,7 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="44.5"/>
@@ -1849,7 +1863,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="24.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="31.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="108.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="108.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="6" style="4" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>

</xml_diff>